<commit_message>
update map understanding project
</commit_message>
<xml_diff>
--- a/code/Legend Analysis/legendAnalysisResultsFinalGood.xlsx
+++ b/code/Legend Analysis/legendAnalysisResultsFinalGood.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\MapElementDetection\code\Legend Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B00E596-12D4-4094-A4DD-77B49D63624D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7FE39-FC4B-483D-BD0F-2753C614ED22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{EBA64443-21D4-4C5B-81AF-29B7215ABC21}"/>
   </bookViews>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB103C9-CAA0-40D2-9C3C-59F04337F69D}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2428,12 +2428,12 @@
         <v>0.48276862026862022</v>
       </c>
       <c r="F80" cm="1">
-        <f t="array" ref="F80">AVERAGE(IF(ISERROR(F2:F79),"",F2:F79))</f>
-        <v>0.89950980392156865</v>
+        <f t="array" ref="F80">AVERAGE(IF(ISERROR(E2:E72),"",E2:E72))</f>
+        <v>0.49844064386317904</v>
       </c>
       <c r="G80">
         <f>2*E80*F80/(E80+F80)</f>
-        <v>0.6283178545765441</v>
+        <v>0.4904794740937285</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>